<commit_message>
documentação atualizada e diário de bordo atualizado
</commit_message>
<xml_diff>
--- a/diario_de_bordo/Diario de Bordo.xlsx
+++ b/diario_de_bordo/Diario de Bordo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\codesphp\dev\pi-segundo-semestre-2025\diario_de_bordo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{012A82CB-B932-4F97-8297-F87C35D73DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152CE058-FF4C-4D4D-9A77-8B4CE689453A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Diário de Bordo" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>DIARIO DE BORDO - NEXBIT</t>
   </si>
@@ -100,6 +100,36 @@
   </si>
   <si>
     <t>Implementação de Pagina de Login/Atualização Documentação</t>
+  </si>
+  <si>
+    <t>Inicio da criação do dashboard, página inicial da aplicação</t>
+  </si>
+  <si>
+    <t>Algumas correções e criação dos gráficos interativos</t>
+  </si>
+  <si>
+    <t>Criação da footer da empresa e tratamento de rotas inacessíveis</t>
+  </si>
+  <si>
+    <t>Documentação do código e refatoração de algumas partes, bem como a troca do fetch api para o axios - Dashboard completa, criação de KPIS e definiçaõ dos mesmos e pequenas atualizações na footer da empresa</t>
+  </si>
+  <si>
+    <t>Inicio da criação da página de clientes e personalizando o UX, tornando o redirecionamento para a página inicial automático.</t>
+  </si>
+  <si>
+    <t>Página de clientes completa, primeiro CRUD funcionando, backend e frontend completos</t>
+  </si>
+  <si>
+    <t>Personalizando o UX, adicionando validação no formulário de cadastro e de update de clientes e pequenas alterações no visual</t>
+  </si>
+  <si>
+    <t>Criação do painel do usuário - Apenas o frontend</t>
+  </si>
+  <si>
+    <t>Adicionando links aos diagramas dentro do repositório, para melhor navegação</t>
+  </si>
+  <si>
+    <t>Inicio da criação da página de motos</t>
   </si>
 </sst>
 </file>
@@ -280,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -324,6 +354,15 @@
     <xf numFmtId="14" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -351,12 +390,14 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -696,10 +737,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="G3:S66"/>
+  <dimension ref="G3:S87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <selection activeCell="R46" sqref="R46"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="L64" sqref="L64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,84 +761,84 @@
   </cols>
   <sheetData>
     <row r="3" spans="7:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="19"/>
-      <c r="R3" s="19"/>
-      <c r="S3" s="19"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22"/>
     </row>
     <row r="4" spans="7:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G4" s="20"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="21"/>
-      <c r="N4" s="21"/>
-      <c r="O4" s="21"/>
-      <c r="P4" s="21"/>
-      <c r="Q4" s="21"/>
-      <c r="R4" s="21"/>
-      <c r="S4" s="21"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="24"/>
+      <c r="S4" s="24"/>
     </row>
     <row r="5" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="23" t="s">
+      <c r="H5" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23" t="s">
+      <c r="I5" s="26"/>
+      <c r="J5" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23" t="s">
+      <c r="K5" s="26"/>
+      <c r="L5" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23" t="s">
+      <c r="M5" s="26"/>
+      <c r="N5" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="O5" s="23"/>
-      <c r="P5" s="15" t="s">
+      <c r="O5" s="26"/>
+      <c r="P5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="Q5" s="15" t="s">
+      <c r="Q5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="R5" s="15" t="s">
+      <c r="R5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="S5" s="17" t="s">
+      <c r="S5" s="20" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="7:19" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G6" s="22"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="16"/>
-      <c r="S6" s="17"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="20"/>
     </row>
     <row r="7" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G7" s="2">
@@ -1550,7 +1591,7 @@
       <c r="I46" s="3"/>
       <c r="J46" s="3"/>
       <c r="K46" s="3"/>
-      <c r="L46" s="24">
+      <c r="L46" s="15">
         <v>45940</v>
       </c>
       <c r="M46" s="3"/>
@@ -1560,7 +1601,7 @@
       </c>
       <c r="P46" s="5"/>
       <c r="Q46" s="9"/>
-      <c r="R46" s="25" t="s">
+      <c r="R46" s="16" t="s">
         <v>24</v>
       </c>
       <c r="S46" s="13" t="s">
@@ -1624,13 +1665,19 @@
       </c>
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
-      <c r="J50" s="3"/>
-      <c r="K50" s="3"/>
+      <c r="J50" s="4">
+        <v>45944</v>
+      </c>
+      <c r="K50" s="4">
+        <v>45944</v>
+      </c>
       <c r="L50" s="3"/>
       <c r="M50" s="3"/>
       <c r="N50" s="3"/>
       <c r="O50" s="3"/>
-      <c r="P50" s="5"/>
+      <c r="P50" s="6" t="s">
+        <v>25</v>
+      </c>
       <c r="Q50" s="9"/>
       <c r="R50" s="5"/>
       <c r="S50" s="5"/>
@@ -1641,64 +1688,88 @@
       </c>
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
-      <c r="K51" s="3"/>
+      <c r="J51" s="4">
+        <v>45945</v>
+      </c>
+      <c r="K51" s="4">
+        <v>45945</v>
+      </c>
       <c r="L51" s="3"/>
       <c r="M51" s="3"/>
       <c r="N51" s="3"/>
       <c r="O51" s="3"/>
-      <c r="P51" s="5"/>
+      <c r="P51" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="Q51" s="9"/>
       <c r="R51" s="5"/>
       <c r="S51" s="5"/>
     </row>
-    <row r="52" spans="7:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="7:19" ht="30" x14ac:dyDescent="0.25">
       <c r="G52" s="2">
         <v>45946</v>
       </c>
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
-      <c r="J52" s="3"/>
-      <c r="K52" s="3"/>
+      <c r="J52" s="17">
+        <v>45946</v>
+      </c>
+      <c r="K52" s="4">
+        <v>45946</v>
+      </c>
       <c r="L52" s="3"/>
       <c r="M52" s="3"/>
       <c r="N52" s="3"/>
       <c r="O52" s="3"/>
-      <c r="P52" s="5"/>
+      <c r="P52" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="Q52" s="9"/>
       <c r="R52" s="5"/>
       <c r="S52" s="5"/>
     </row>
-    <row r="53" spans="7:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="7:19" ht="60" x14ac:dyDescent="0.25">
       <c r="G53" s="2">
         <v>45947</v>
       </c>
       <c r="H53" s="3"/>
       <c r="I53" s="3"/>
-      <c r="J53" s="3"/>
-      <c r="K53" s="3"/>
+      <c r="J53" s="4">
+        <v>45947</v>
+      </c>
+      <c r="K53" s="4">
+        <v>45947</v>
+      </c>
       <c r="L53" s="3"/>
       <c r="M53" s="3"/>
       <c r="N53" s="3"/>
       <c r="O53" s="3"/>
-      <c r="P53" s="5"/>
+      <c r="P53" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="Q53" s="9"/>
       <c r="R53" s="5"/>
       <c r="S53" s="5"/>
     </row>
-    <row r="54" spans="7:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="7:19" ht="45" x14ac:dyDescent="0.25">
       <c r="G54" s="2">
         <v>45948</v>
       </c>
       <c r="H54" s="3"/>
       <c r="I54" s="3"/>
-      <c r="J54" s="3"/>
-      <c r="K54" s="3"/>
+      <c r="J54" s="4">
+        <v>45948</v>
+      </c>
+      <c r="K54" s="4">
+        <v>45948</v>
+      </c>
       <c r="L54" s="3"/>
       <c r="M54" s="3"/>
       <c r="N54" s="3"/>
       <c r="O54" s="3"/>
-      <c r="P54" s="5"/>
+      <c r="P54" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="Q54" s="9"/>
       <c r="R54" s="5"/>
       <c r="S54" s="5"/>
@@ -1737,19 +1808,25 @@
       <c r="R56" s="5"/>
       <c r="S56" s="5"/>
     </row>
-    <row r="57" spans="7:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="7:19" ht="30" x14ac:dyDescent="0.25">
       <c r="G57" s="2">
         <v>45951</v>
       </c>
       <c r="H57" s="3"/>
       <c r="I57" s="3"/>
-      <c r="J57" s="3"/>
-      <c r="K57" s="3"/>
+      <c r="J57" s="4">
+        <v>45951</v>
+      </c>
+      <c r="K57" s="4">
+        <v>45951</v>
+      </c>
       <c r="L57" s="3"/>
       <c r="M57" s="3"/>
       <c r="N57" s="3"/>
       <c r="O57" s="3"/>
-      <c r="P57" s="5"/>
+      <c r="P57" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="Q57" s="9"/>
       <c r="R57" s="5"/>
       <c r="S57" s="5"/>
@@ -1771,19 +1848,25 @@
       <c r="R58" s="5"/>
       <c r="S58" s="5"/>
     </row>
-    <row r="59" spans="7:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="7:19" ht="45" x14ac:dyDescent="0.25">
       <c r="G59" s="2">
         <v>45953</v>
       </c>
       <c r="H59" s="3"/>
       <c r="I59" s="3"/>
-      <c r="J59" s="3"/>
-      <c r="K59" s="3"/>
+      <c r="J59" s="4">
+        <v>45953</v>
+      </c>
+      <c r="K59" s="4">
+        <v>45953</v>
+      </c>
       <c r="L59" s="3"/>
       <c r="M59" s="3"/>
       <c r="N59" s="3"/>
       <c r="O59" s="3"/>
-      <c r="P59" s="5"/>
+      <c r="P59" s="6" t="s">
+        <v>31</v>
+      </c>
       <c r="Q59" s="9"/>
       <c r="R59" s="5"/>
       <c r="S59" s="5"/>
@@ -1794,13 +1877,19 @@
       </c>
       <c r="H60" s="3"/>
       <c r="I60" s="3"/>
-      <c r="J60" s="3"/>
-      <c r="K60" s="3"/>
+      <c r="J60" s="4">
+        <v>45954</v>
+      </c>
+      <c r="K60" s="4">
+        <v>45954</v>
+      </c>
       <c r="L60" s="3"/>
       <c r="M60" s="3"/>
       <c r="N60" s="3"/>
       <c r="O60" s="3"/>
-      <c r="P60" s="5"/>
+      <c r="P60" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="Q60" s="9"/>
       <c r="R60" s="5"/>
       <c r="S60" s="5"/>
@@ -1873,19 +1962,25 @@
       <c r="R64" s="5"/>
       <c r="S64" s="5"/>
     </row>
-    <row r="65" spans="7:19" x14ac:dyDescent="0.25">
+    <row r="65" spans="7:19" ht="30" x14ac:dyDescent="0.25">
       <c r="G65" s="2">
         <v>45959</v>
       </c>
       <c r="H65" s="3"/>
       <c r="I65" s="3"/>
-      <c r="J65" s="3"/>
-      <c r="K65" s="3"/>
+      <c r="J65" s="4">
+        <v>45959</v>
+      </c>
+      <c r="K65" s="4">
+        <v>45959</v>
+      </c>
       <c r="L65" s="3"/>
       <c r="M65" s="3"/>
       <c r="N65" s="3"/>
       <c r="O65" s="3"/>
-      <c r="P65" s="5"/>
+      <c r="P65" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="Q65" s="9"/>
       <c r="R65" s="5"/>
       <c r="S65" s="5"/>
@@ -1906,6 +2001,369 @@
       <c r="Q66" s="9"/>
       <c r="R66" s="5"/>
       <c r="S66" s="5"/>
+    </row>
+    <row r="67" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="G67" s="28">
+        <v>45961</v>
+      </c>
+      <c r="H67" s="29"/>
+      <c r="I67" s="29"/>
+      <c r="J67" s="30">
+        <v>45961</v>
+      </c>
+      <c r="K67" s="30">
+        <v>45961</v>
+      </c>
+      <c r="L67" s="29"/>
+      <c r="M67" s="29"/>
+      <c r="N67" s="29"/>
+      <c r="O67" s="29"/>
+      <c r="P67" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q67" s="29"/>
+      <c r="R67" s="29"/>
+      <c r="S67" s="29"/>
+    </row>
+    <row r="68" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="G68" s="28">
+        <v>45962</v>
+      </c>
+      <c r="H68" s="29"/>
+      <c r="I68" s="29"/>
+      <c r="J68" s="29"/>
+      <c r="K68" s="29"/>
+      <c r="L68" s="29"/>
+      <c r="M68" s="29"/>
+      <c r="N68" s="29"/>
+      <c r="O68" s="29"/>
+      <c r="P68" s="27"/>
+      <c r="Q68" s="29"/>
+      <c r="R68" s="29"/>
+      <c r="S68" s="29"/>
+    </row>
+    <row r="69" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="G69" s="28">
+        <v>45963</v>
+      </c>
+      <c r="H69" s="29"/>
+      <c r="I69" s="29"/>
+      <c r="J69" s="29"/>
+      <c r="K69" s="29"/>
+      <c r="L69" s="29"/>
+      <c r="M69" s="29"/>
+      <c r="N69" s="29"/>
+      <c r="O69" s="29"/>
+      <c r="P69" s="27"/>
+      <c r="Q69" s="29"/>
+      <c r="R69" s="29"/>
+      <c r="S69" s="29"/>
+    </row>
+    <row r="70" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="G70" s="28">
+        <v>45964</v>
+      </c>
+      <c r="H70" s="29"/>
+      <c r="I70" s="29"/>
+      <c r="J70" s="29"/>
+      <c r="K70" s="29"/>
+      <c r="L70" s="29"/>
+      <c r="M70" s="29"/>
+      <c r="N70" s="29"/>
+      <c r="O70" s="29"/>
+      <c r="P70" s="27"/>
+      <c r="Q70" s="29"/>
+      <c r="R70" s="29"/>
+      <c r="S70" s="29"/>
+    </row>
+    <row r="71" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="G71" s="28">
+        <v>45965</v>
+      </c>
+      <c r="H71" s="29"/>
+      <c r="I71" s="29"/>
+      <c r="J71" s="29"/>
+      <c r="K71" s="29"/>
+      <c r="L71" s="29"/>
+      <c r="M71" s="29"/>
+      <c r="N71" s="29"/>
+      <c r="O71" s="29"/>
+      <c r="P71" s="27"/>
+      <c r="Q71" s="29"/>
+      <c r="R71" s="29"/>
+      <c r="S71" s="29"/>
+    </row>
+    <row r="72" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="G72" s="28">
+        <v>45966</v>
+      </c>
+      <c r="H72" s="29"/>
+      <c r="I72" s="29"/>
+      <c r="J72" s="29"/>
+      <c r="K72" s="29"/>
+      <c r="L72" s="29"/>
+      <c r="M72" s="29"/>
+      <c r="N72" s="29"/>
+      <c r="O72" s="29"/>
+      <c r="P72" s="27"/>
+      <c r="Q72" s="29"/>
+      <c r="R72" s="29"/>
+      <c r="S72" s="29"/>
+    </row>
+    <row r="73" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="G73" s="28">
+        <v>45967</v>
+      </c>
+      <c r="H73" s="29"/>
+      <c r="I73" s="29"/>
+      <c r="J73" s="29"/>
+      <c r="K73" s="29"/>
+      <c r="L73" s="29"/>
+      <c r="M73" s="29"/>
+      <c r="N73" s="29"/>
+      <c r="O73" s="29"/>
+      <c r="P73" s="27"/>
+      <c r="Q73" s="29"/>
+      <c r="R73" s="29"/>
+      <c r="S73" s="29"/>
+    </row>
+    <row r="74" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="G74" s="28">
+        <v>45968</v>
+      </c>
+      <c r="H74" s="29"/>
+      <c r="I74" s="29"/>
+      <c r="J74" s="29"/>
+      <c r="K74" s="29"/>
+      <c r="L74" s="29"/>
+      <c r="M74" s="29"/>
+      <c r="N74" s="29"/>
+      <c r="O74" s="29"/>
+      <c r="P74" s="27"/>
+      <c r="Q74" s="29"/>
+      <c r="R74" s="29"/>
+      <c r="S74" s="29"/>
+    </row>
+    <row r="75" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="G75" s="28">
+        <v>45969</v>
+      </c>
+      <c r="H75" s="29"/>
+      <c r="I75" s="29"/>
+      <c r="J75" s="29"/>
+      <c r="K75" s="29"/>
+      <c r="L75" s="29"/>
+      <c r="M75" s="29"/>
+      <c r="N75" s="29"/>
+      <c r="O75" s="29"/>
+      <c r="P75" s="27"/>
+      <c r="Q75" s="29"/>
+      <c r="R75" s="29"/>
+      <c r="S75" s="29"/>
+    </row>
+    <row r="76" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="G76" s="28">
+        <v>45970</v>
+      </c>
+      <c r="H76" s="29"/>
+      <c r="I76" s="29"/>
+      <c r="J76" s="29"/>
+      <c r="K76" s="29"/>
+      <c r="L76" s="29"/>
+      <c r="M76" s="29"/>
+      <c r="N76" s="29"/>
+      <c r="O76" s="29"/>
+      <c r="P76" s="27"/>
+      <c r="Q76" s="29"/>
+      <c r="R76" s="29"/>
+      <c r="S76" s="29"/>
+    </row>
+    <row r="77" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="G77" s="28">
+        <v>45971</v>
+      </c>
+      <c r="H77" s="29"/>
+      <c r="I77" s="29"/>
+      <c r="J77" s="29"/>
+      <c r="K77" s="29"/>
+      <c r="L77" s="29"/>
+      <c r="M77" s="29"/>
+      <c r="N77" s="29"/>
+      <c r="O77" s="29"/>
+      <c r="P77" s="27"/>
+      <c r="Q77" s="29"/>
+      <c r="R77" s="29"/>
+      <c r="S77" s="29"/>
+    </row>
+    <row r="78" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="G78" s="28">
+        <v>45972</v>
+      </c>
+      <c r="H78" s="29"/>
+      <c r="I78" s="29"/>
+      <c r="J78" s="29"/>
+      <c r="K78" s="29"/>
+      <c r="L78" s="29"/>
+      <c r="M78" s="29"/>
+      <c r="N78" s="29"/>
+      <c r="O78" s="29"/>
+      <c r="P78" s="27"/>
+      <c r="Q78" s="29"/>
+      <c r="R78" s="29"/>
+      <c r="S78" s="29"/>
+    </row>
+    <row r="79" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="G79" s="28">
+        <v>45973</v>
+      </c>
+      <c r="H79" s="29"/>
+      <c r="I79" s="29"/>
+      <c r="J79" s="29"/>
+      <c r="K79" s="29"/>
+      <c r="L79" s="29"/>
+      <c r="M79" s="29"/>
+      <c r="N79" s="29"/>
+      <c r="O79" s="29"/>
+      <c r="P79" s="27"/>
+      <c r="Q79" s="29"/>
+      <c r="R79" s="29"/>
+      <c r="S79" s="29"/>
+    </row>
+    <row r="80" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="G80" s="28">
+        <v>45974</v>
+      </c>
+      <c r="H80" s="29"/>
+      <c r="I80" s="29"/>
+      <c r="J80" s="29"/>
+      <c r="K80" s="29"/>
+      <c r="L80" s="29"/>
+      <c r="M80" s="29"/>
+      <c r="N80" s="29"/>
+      <c r="O80" s="29"/>
+      <c r="P80" s="27"/>
+      <c r="Q80" s="29"/>
+      <c r="R80" s="29"/>
+      <c r="S80" s="29"/>
+    </row>
+    <row r="81" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="G81" s="28">
+        <v>45975</v>
+      </c>
+      <c r="H81" s="29"/>
+      <c r="I81" s="29"/>
+      <c r="J81" s="29"/>
+      <c r="K81" s="29"/>
+      <c r="L81" s="29"/>
+      <c r="M81" s="29"/>
+      <c r="N81" s="29"/>
+      <c r="O81" s="29"/>
+      <c r="P81" s="27"/>
+      <c r="Q81" s="29"/>
+      <c r="R81" s="29"/>
+      <c r="S81" s="29"/>
+    </row>
+    <row r="82" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="G82" s="28">
+        <v>45976</v>
+      </c>
+      <c r="H82" s="29"/>
+      <c r="I82" s="29"/>
+      <c r="J82" s="29"/>
+      <c r="K82" s="29"/>
+      <c r="L82" s="29"/>
+      <c r="M82" s="29"/>
+      <c r="N82" s="29"/>
+      <c r="O82" s="29"/>
+      <c r="P82" s="27"/>
+      <c r="Q82" s="29"/>
+      <c r="R82" s="29"/>
+      <c r="S82" s="29"/>
+    </row>
+    <row r="83" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="G83" s="28">
+        <v>45977</v>
+      </c>
+      <c r="H83" s="29"/>
+      <c r="I83" s="29"/>
+      <c r="J83" s="29"/>
+      <c r="K83" s="29"/>
+      <c r="L83" s="29"/>
+      <c r="M83" s="29"/>
+      <c r="N83" s="29"/>
+      <c r="O83" s="29"/>
+      <c r="P83" s="27"/>
+      <c r="Q83" s="29"/>
+      <c r="R83" s="29"/>
+      <c r="S83" s="29"/>
+    </row>
+    <row r="84" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="G84" s="28">
+        <v>45978</v>
+      </c>
+      <c r="H84" s="29"/>
+      <c r="I84" s="29"/>
+      <c r="J84" s="29"/>
+      <c r="K84" s="29"/>
+      <c r="L84" s="29"/>
+      <c r="M84" s="29"/>
+      <c r="N84" s="29"/>
+      <c r="O84" s="29"/>
+      <c r="P84" s="27"/>
+      <c r="Q84" s="29"/>
+      <c r="R84" s="29"/>
+      <c r="S84" s="29"/>
+    </row>
+    <row r="85" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="G85" s="28">
+        <v>45979</v>
+      </c>
+      <c r="H85" s="29"/>
+      <c r="I85" s="29"/>
+      <c r="J85" s="29"/>
+      <c r="K85" s="29"/>
+      <c r="L85" s="29"/>
+      <c r="M85" s="29"/>
+      <c r="N85" s="29"/>
+      <c r="O85" s="29"/>
+      <c r="P85" s="27"/>
+      <c r="Q85" s="29"/>
+      <c r="R85" s="29"/>
+      <c r="S85" s="29"/>
+    </row>
+    <row r="86" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="G86" s="28">
+        <v>45980</v>
+      </c>
+      <c r="H86" s="29"/>
+      <c r="I86" s="29"/>
+      <c r="J86" s="29"/>
+      <c r="K86" s="29"/>
+      <c r="L86" s="29"/>
+      <c r="M86" s="29"/>
+      <c r="N86" s="29"/>
+      <c r="O86" s="29"/>
+      <c r="P86" s="27"/>
+      <c r="Q86" s="29"/>
+      <c r="R86" s="29"/>
+      <c r="S86" s="29"/>
+    </row>
+    <row r="87" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="G87" s="28">
+        <v>45981</v>
+      </c>
+      <c r="H87" s="29"/>
+      <c r="I87" s="29"/>
+      <c r="J87" s="29"/>
+      <c r="K87" s="29"/>
+      <c r="L87" s="29"/>
+      <c r="M87" s="29"/>
+      <c r="N87" s="29"/>
+      <c r="O87" s="29"/>
+      <c r="P87" s="27"/>
+      <c r="Q87" s="29"/>
+      <c r="R87" s="29"/>
+      <c r="S87" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>

<commit_message>
Implementa documentação 4.5 e atualiza diario de bordo
</commit_message>
<xml_diff>
--- a/diario_de_bordo/Diario de Bordo.xlsx
+++ b/diario_de_bordo/Diario de Bordo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\codesphp\dev\pi-segundo-semestre-2025\diario_de_bordo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\pi-2\pi-segundo-semestre-2025\diario_de_bordo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{152CE058-FF4C-4D4D-9A77-8B4CE689453A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C6AA95-83AE-4751-9A84-639EA8FCC78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Diário de Bordo" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>DIARIO DE BORDO - NEXBIT</t>
   </si>
@@ -130,6 +130,12 @@
   </si>
   <si>
     <t>Inicio da criação da página de motos</t>
+  </si>
+  <si>
+    <t>Documentação 4.5 feita e restruturação de backend de login.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagrama de classe feito pronto para avaliação </t>
   </si>
 </sst>
 </file>
@@ -363,6 +369,14 @@
     <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -390,14 +404,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -739,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="G3:S87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="L64" sqref="L64"/>
+    <sheetView tabSelected="1" topLeftCell="E52" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="R75" sqref="R75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -761,84 +767,84 @@
   </cols>
   <sheetData>
     <row r="3" spans="7:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="22"/>
-      <c r="P3" s="22"/>
-      <c r="Q3" s="22"/>
-      <c r="R3" s="22"/>
-      <c r="S3" s="22"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="26"/>
+      <c r="R3" s="26"/>
+      <c r="S3" s="26"/>
     </row>
     <row r="4" spans="7:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G4" s="23"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="24"/>
-      <c r="O4" s="24"/>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="24"/>
-      <c r="R4" s="24"/>
-      <c r="S4" s="24"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="28"/>
+      <c r="Q4" s="28"/>
+      <c r="R4" s="28"/>
+      <c r="S4" s="28"/>
     </row>
     <row r="5" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G5" s="25" t="s">
+      <c r="G5" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="26" t="s">
+      <c r="H5" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26" t="s">
+      <c r="I5" s="30"/>
+      <c r="J5" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="26"/>
-      <c r="L5" s="26" t="s">
+      <c r="K5" s="30"/>
+      <c r="L5" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26" t="s">
+      <c r="M5" s="30"/>
+      <c r="N5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="O5" s="26"/>
-      <c r="P5" s="18" t="s">
+      <c r="O5" s="30"/>
+      <c r="P5" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="Q5" s="18" t="s">
+      <c r="Q5" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="R5" s="18" t="s">
+      <c r="R5" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="S5" s="20" t="s">
+      <c r="S5" s="24" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="7:19" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G6" s="25"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
-      <c r="N6" s="26"/>
-      <c r="O6" s="26"/>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="19"/>
-      <c r="R6" s="19"/>
-      <c r="S6" s="20"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="30"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="24"/>
     </row>
     <row r="7" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G7" s="2">
@@ -2003,367 +2009,375 @@
       <c r="S66" s="5"/>
     </row>
     <row r="67" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G67" s="28">
+      <c r="G67" s="19">
         <v>45961</v>
       </c>
-      <c r="H67" s="29"/>
-      <c r="I67" s="29"/>
-      <c r="J67" s="30">
+      <c r="H67" s="20"/>
+      <c r="I67" s="20"/>
+      <c r="J67" s="21">
         <v>45961</v>
       </c>
-      <c r="K67" s="30">
+      <c r="K67" s="21">
         <v>45961</v>
       </c>
-      <c r="L67" s="29"/>
-      <c r="M67" s="29"/>
-      <c r="N67" s="29"/>
-      <c r="O67" s="29"/>
+      <c r="L67" s="20"/>
+      <c r="M67" s="20"/>
+      <c r="N67" s="20"/>
+      <c r="O67" s="20"/>
       <c r="P67" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="Q67" s="29"/>
-      <c r="R67" s="29"/>
-      <c r="S67" s="29"/>
+      <c r="Q67" s="20"/>
+      <c r="R67" s="20"/>
+      <c r="S67" s="20"/>
     </row>
     <row r="68" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G68" s="28">
+      <c r="G68" s="19">
         <v>45962</v>
       </c>
-      <c r="H68" s="29"/>
-      <c r="I68" s="29"/>
-      <c r="J68" s="29"/>
-      <c r="K68" s="29"/>
-      <c r="L68" s="29"/>
-      <c r="M68" s="29"/>
-      <c r="N68" s="29"/>
-      <c r="O68" s="29"/>
-      <c r="P68" s="27"/>
-      <c r="Q68" s="29"/>
-      <c r="R68" s="29"/>
-      <c r="S68" s="29"/>
+      <c r="H68" s="20"/>
+      <c r="I68" s="20"/>
+      <c r="J68" s="20"/>
+      <c r="K68" s="20"/>
+      <c r="L68" s="20"/>
+      <c r="M68" s="20"/>
+      <c r="N68" s="20"/>
+      <c r="O68" s="20"/>
+      <c r="P68" s="18"/>
+      <c r="Q68" s="20"/>
+      <c r="R68" s="20"/>
+      <c r="S68" s="20"/>
     </row>
     <row r="69" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G69" s="28">
+      <c r="G69" s="19">
         <v>45963</v>
       </c>
-      <c r="H69" s="29"/>
-      <c r="I69" s="29"/>
-      <c r="J69" s="29"/>
-      <c r="K69" s="29"/>
-      <c r="L69" s="29"/>
-      <c r="M69" s="29"/>
-      <c r="N69" s="29"/>
-      <c r="O69" s="29"/>
-      <c r="P69" s="27"/>
-      <c r="Q69" s="29"/>
-      <c r="R69" s="29"/>
-      <c r="S69" s="29"/>
+      <c r="H69" s="20"/>
+      <c r="I69" s="20"/>
+      <c r="J69" s="20"/>
+      <c r="K69" s="20"/>
+      <c r="L69" s="20"/>
+      <c r="M69" s="20"/>
+      <c r="N69" s="20"/>
+      <c r="O69" s="20"/>
+      <c r="P69" s="18"/>
+      <c r="Q69" s="20"/>
+      <c r="R69" s="20"/>
+      <c r="S69" s="20"/>
     </row>
     <row r="70" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G70" s="28">
+      <c r="G70" s="19">
         <v>45964</v>
       </c>
-      <c r="H70" s="29"/>
-      <c r="I70" s="29"/>
-      <c r="J70" s="29"/>
-      <c r="K70" s="29"/>
-      <c r="L70" s="29"/>
-      <c r="M70" s="29"/>
-      <c r="N70" s="29"/>
-      <c r="O70" s="29"/>
-      <c r="P70" s="27"/>
-      <c r="Q70" s="29"/>
-      <c r="R70" s="29"/>
-      <c r="S70" s="29"/>
-    </row>
-    <row r="71" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G71" s="28">
+      <c r="H70" s="20"/>
+      <c r="I70" s="20"/>
+      <c r="J70" s="20"/>
+      <c r="K70" s="20"/>
+      <c r="L70" s="20"/>
+      <c r="M70" s="20"/>
+      <c r="N70" s="20"/>
+      <c r="O70" s="20"/>
+      <c r="P70" s="18"/>
+      <c r="Q70" s="20"/>
+      <c r="R70" s="20"/>
+      <c r="S70" s="20"/>
+    </row>
+    <row r="71" spans="7:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="G71" s="19">
         <v>45965</v>
       </c>
-      <c r="H71" s="29"/>
-      <c r="I71" s="29"/>
-      <c r="J71" s="29"/>
-      <c r="K71" s="29"/>
-      <c r="L71" s="29"/>
-      <c r="M71" s="29"/>
-      <c r="N71" s="29"/>
-      <c r="O71" s="29"/>
-      <c r="P71" s="27"/>
-      <c r="Q71" s="29"/>
-      <c r="R71" s="29"/>
-      <c r="S71" s="29"/>
-    </row>
-    <row r="72" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G72" s="28">
+      <c r="H71" s="20"/>
+      <c r="I71" s="20"/>
+      <c r="J71" s="20"/>
+      <c r="K71" s="20"/>
+      <c r="L71" s="15">
+        <v>45965</v>
+      </c>
+      <c r="M71" s="20"/>
+      <c r="N71" s="20"/>
+      <c r="O71" s="20"/>
+      <c r="P71" s="18"/>
+      <c r="Q71" s="20"/>
+      <c r="R71" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="S71" s="20"/>
+    </row>
+    <row r="72" spans="7:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="G72" s="19">
         <v>45966</v>
       </c>
-      <c r="H72" s="29"/>
-      <c r="I72" s="29"/>
-      <c r="J72" s="29"/>
-      <c r="K72" s="29"/>
-      <c r="L72" s="29"/>
-      <c r="M72" s="29"/>
-      <c r="N72" s="29"/>
-      <c r="O72" s="29"/>
-      <c r="P72" s="27"/>
-      <c r="Q72" s="29"/>
-      <c r="R72" s="29"/>
-      <c r="S72" s="29"/>
+      <c r="H72" s="20"/>
+      <c r="I72" s="20"/>
+      <c r="J72" s="20"/>
+      <c r="K72" s="20"/>
+      <c r="L72" s="15">
+        <v>45966</v>
+      </c>
+      <c r="M72" s="20"/>
+      <c r="N72" s="20"/>
+      <c r="O72" s="20"/>
+      <c r="P72" s="18"/>
+      <c r="Q72" s="20"/>
+      <c r="R72" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="S72" s="20"/>
     </row>
     <row r="73" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G73" s="28">
+      <c r="G73" s="19">
         <v>45967</v>
       </c>
-      <c r="H73" s="29"/>
-      <c r="I73" s="29"/>
-      <c r="J73" s="29"/>
-      <c r="K73" s="29"/>
-      <c r="L73" s="29"/>
-      <c r="M73" s="29"/>
-      <c r="N73" s="29"/>
-      <c r="O73" s="29"/>
-      <c r="P73" s="27"/>
-      <c r="Q73" s="29"/>
-      <c r="R73" s="29"/>
-      <c r="S73" s="29"/>
+      <c r="H73" s="20"/>
+      <c r="I73" s="20"/>
+      <c r="J73" s="20"/>
+      <c r="K73" s="20"/>
+      <c r="L73" s="20"/>
+      <c r="M73" s="20"/>
+      <c r="N73" s="20"/>
+      <c r="O73" s="20"/>
+      <c r="P73" s="18"/>
+      <c r="Q73" s="20"/>
+      <c r="R73" s="20"/>
+      <c r="S73" s="20"/>
     </row>
     <row r="74" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G74" s="28">
+      <c r="G74" s="19">
         <v>45968</v>
       </c>
-      <c r="H74" s="29"/>
-      <c r="I74" s="29"/>
-      <c r="J74" s="29"/>
-      <c r="K74" s="29"/>
-      <c r="L74" s="29"/>
-      <c r="M74" s="29"/>
-      <c r="N74" s="29"/>
-      <c r="O74" s="29"/>
-      <c r="P74" s="27"/>
-      <c r="Q74" s="29"/>
-      <c r="R74" s="29"/>
-      <c r="S74" s="29"/>
+      <c r="H74" s="20"/>
+      <c r="I74" s="20"/>
+      <c r="J74" s="20"/>
+      <c r="K74" s="20"/>
+      <c r="L74" s="20"/>
+      <c r="M74" s="20"/>
+      <c r="N74" s="20"/>
+      <c r="O74" s="20"/>
+      <c r="P74" s="18"/>
+      <c r="Q74" s="20"/>
+      <c r="R74" s="20"/>
+      <c r="S74" s="20"/>
     </row>
     <row r="75" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G75" s="28">
+      <c r="G75" s="19">
         <v>45969</v>
       </c>
-      <c r="H75" s="29"/>
-      <c r="I75" s="29"/>
-      <c r="J75" s="29"/>
-      <c r="K75" s="29"/>
-      <c r="L75" s="29"/>
-      <c r="M75" s="29"/>
-      <c r="N75" s="29"/>
-      <c r="O75" s="29"/>
-      <c r="P75" s="27"/>
-      <c r="Q75" s="29"/>
-      <c r="R75" s="29"/>
-      <c r="S75" s="29"/>
+      <c r="H75" s="20"/>
+      <c r="I75" s="20"/>
+      <c r="J75" s="20"/>
+      <c r="K75" s="20"/>
+      <c r="L75" s="20"/>
+      <c r="M75" s="20"/>
+      <c r="N75" s="20"/>
+      <c r="O75" s="20"/>
+      <c r="P75" s="18"/>
+      <c r="Q75" s="20"/>
+      <c r="R75" s="20"/>
+      <c r="S75" s="20"/>
     </row>
     <row r="76" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G76" s="28">
+      <c r="G76" s="19">
         <v>45970</v>
       </c>
-      <c r="H76" s="29"/>
-      <c r="I76" s="29"/>
-      <c r="J76" s="29"/>
-      <c r="K76" s="29"/>
-      <c r="L76" s="29"/>
-      <c r="M76" s="29"/>
-      <c r="N76" s="29"/>
-      <c r="O76" s="29"/>
-      <c r="P76" s="27"/>
-      <c r="Q76" s="29"/>
-      <c r="R76" s="29"/>
-      <c r="S76" s="29"/>
+      <c r="H76" s="20"/>
+      <c r="I76" s="20"/>
+      <c r="J76" s="20"/>
+      <c r="K76" s="20"/>
+      <c r="L76" s="20"/>
+      <c r="M76" s="20"/>
+      <c r="N76" s="20"/>
+      <c r="O76" s="20"/>
+      <c r="P76" s="18"/>
+      <c r="Q76" s="20"/>
+      <c r="R76" s="20"/>
+      <c r="S76" s="20"/>
     </row>
     <row r="77" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G77" s="28">
+      <c r="G77" s="19">
         <v>45971</v>
       </c>
-      <c r="H77" s="29"/>
-      <c r="I77" s="29"/>
-      <c r="J77" s="29"/>
-      <c r="K77" s="29"/>
-      <c r="L77" s="29"/>
-      <c r="M77" s="29"/>
-      <c r="N77" s="29"/>
-      <c r="O77" s="29"/>
-      <c r="P77" s="27"/>
-      <c r="Q77" s="29"/>
-      <c r="R77" s="29"/>
-      <c r="S77" s="29"/>
+      <c r="H77" s="20"/>
+      <c r="I77" s="20"/>
+      <c r="J77" s="20"/>
+      <c r="K77" s="20"/>
+      <c r="L77" s="20"/>
+      <c r="M77" s="20"/>
+      <c r="N77" s="20"/>
+      <c r="O77" s="20"/>
+      <c r="P77" s="18"/>
+      <c r="Q77" s="20"/>
+      <c r="R77" s="20"/>
+      <c r="S77" s="20"/>
     </row>
     <row r="78" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G78" s="28">
+      <c r="G78" s="19">
         <v>45972</v>
       </c>
-      <c r="H78" s="29"/>
-      <c r="I78" s="29"/>
-      <c r="J78" s="29"/>
-      <c r="K78" s="29"/>
-      <c r="L78" s="29"/>
-      <c r="M78" s="29"/>
-      <c r="N78" s="29"/>
-      <c r="O78" s="29"/>
-      <c r="P78" s="27"/>
-      <c r="Q78" s="29"/>
-      <c r="R78" s="29"/>
-      <c r="S78" s="29"/>
+      <c r="H78" s="20"/>
+      <c r="I78" s="20"/>
+      <c r="J78" s="20"/>
+      <c r="K78" s="20"/>
+      <c r="L78" s="20"/>
+      <c r="M78" s="20"/>
+      <c r="N78" s="20"/>
+      <c r="O78" s="20"/>
+      <c r="P78" s="18"/>
+      <c r="Q78" s="20"/>
+      <c r="R78" s="20"/>
+      <c r="S78" s="20"/>
     </row>
     <row r="79" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G79" s="28">
+      <c r="G79" s="19">
         <v>45973</v>
       </c>
-      <c r="H79" s="29"/>
-      <c r="I79" s="29"/>
-      <c r="J79" s="29"/>
-      <c r="K79" s="29"/>
-      <c r="L79" s="29"/>
-      <c r="M79" s="29"/>
-      <c r="N79" s="29"/>
-      <c r="O79" s="29"/>
-      <c r="P79" s="27"/>
-      <c r="Q79" s="29"/>
-      <c r="R79" s="29"/>
-      <c r="S79" s="29"/>
+      <c r="H79" s="20"/>
+      <c r="I79" s="20"/>
+      <c r="J79" s="20"/>
+      <c r="K79" s="20"/>
+      <c r="L79" s="20"/>
+      <c r="M79" s="20"/>
+      <c r="N79" s="20"/>
+      <c r="O79" s="20"/>
+      <c r="P79" s="18"/>
+      <c r="Q79" s="20"/>
+      <c r="R79" s="20"/>
+      <c r="S79" s="20"/>
     </row>
     <row r="80" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G80" s="28">
+      <c r="G80" s="19">
         <v>45974</v>
       </c>
-      <c r="H80" s="29"/>
-      <c r="I80" s="29"/>
-      <c r="J80" s="29"/>
-      <c r="K80" s="29"/>
-      <c r="L80" s="29"/>
-      <c r="M80" s="29"/>
-      <c r="N80" s="29"/>
-      <c r="O80" s="29"/>
-      <c r="P80" s="27"/>
-      <c r="Q80" s="29"/>
-      <c r="R80" s="29"/>
-      <c r="S80" s="29"/>
+      <c r="H80" s="20"/>
+      <c r="I80" s="20"/>
+      <c r="J80" s="20"/>
+      <c r="K80" s="20"/>
+      <c r="L80" s="20"/>
+      <c r="M80" s="20"/>
+      <c r="N80" s="20"/>
+      <c r="O80" s="20"/>
+      <c r="P80" s="18"/>
+      <c r="Q80" s="20"/>
+      <c r="R80" s="20"/>
+      <c r="S80" s="20"/>
     </row>
     <row r="81" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G81" s="28">
+      <c r="G81" s="19">
         <v>45975</v>
       </c>
-      <c r="H81" s="29"/>
-      <c r="I81" s="29"/>
-      <c r="J81" s="29"/>
-      <c r="K81" s="29"/>
-      <c r="L81" s="29"/>
-      <c r="M81" s="29"/>
-      <c r="N81" s="29"/>
-      <c r="O81" s="29"/>
-      <c r="P81" s="27"/>
-      <c r="Q81" s="29"/>
-      <c r="R81" s="29"/>
-      <c r="S81" s="29"/>
+      <c r="H81" s="20"/>
+      <c r="I81" s="20"/>
+      <c r="J81" s="20"/>
+      <c r="K81" s="20"/>
+      <c r="L81" s="20"/>
+      <c r="M81" s="20"/>
+      <c r="N81" s="20"/>
+      <c r="O81" s="20"/>
+      <c r="P81" s="18"/>
+      <c r="Q81" s="20"/>
+      <c r="R81" s="20"/>
+      <c r="S81" s="20"/>
     </row>
     <row r="82" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G82" s="28">
+      <c r="G82" s="19">
         <v>45976</v>
       </c>
-      <c r="H82" s="29"/>
-      <c r="I82" s="29"/>
-      <c r="J82" s="29"/>
-      <c r="K82" s="29"/>
-      <c r="L82" s="29"/>
-      <c r="M82" s="29"/>
-      <c r="N82" s="29"/>
-      <c r="O82" s="29"/>
-      <c r="P82" s="27"/>
-      <c r="Q82" s="29"/>
-      <c r="R82" s="29"/>
-      <c r="S82" s="29"/>
+      <c r="H82" s="20"/>
+      <c r="I82" s="20"/>
+      <c r="J82" s="20"/>
+      <c r="K82" s="20"/>
+      <c r="L82" s="20"/>
+      <c r="M82" s="20"/>
+      <c r="N82" s="20"/>
+      <c r="O82" s="20"/>
+      <c r="P82" s="18"/>
+      <c r="Q82" s="20"/>
+      <c r="R82" s="20"/>
+      <c r="S82" s="20"/>
     </row>
     <row r="83" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G83" s="28">
+      <c r="G83" s="19">
         <v>45977</v>
       </c>
-      <c r="H83" s="29"/>
-      <c r="I83" s="29"/>
-      <c r="J83" s="29"/>
-      <c r="K83" s="29"/>
-      <c r="L83" s="29"/>
-      <c r="M83" s="29"/>
-      <c r="N83" s="29"/>
-      <c r="O83" s="29"/>
-      <c r="P83" s="27"/>
-      <c r="Q83" s="29"/>
-      <c r="R83" s="29"/>
-      <c r="S83" s="29"/>
+      <c r="H83" s="20"/>
+      <c r="I83" s="20"/>
+      <c r="J83" s="20"/>
+      <c r="K83" s="20"/>
+      <c r="L83" s="20"/>
+      <c r="M83" s="20"/>
+      <c r="N83" s="20"/>
+      <c r="O83" s="20"/>
+      <c r="P83" s="18"/>
+      <c r="Q83" s="20"/>
+      <c r="R83" s="20"/>
+      <c r="S83" s="20"/>
     </row>
     <row r="84" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G84" s="28">
+      <c r="G84" s="19">
         <v>45978</v>
       </c>
-      <c r="H84" s="29"/>
-      <c r="I84" s="29"/>
-      <c r="J84" s="29"/>
-      <c r="K84" s="29"/>
-      <c r="L84" s="29"/>
-      <c r="M84" s="29"/>
-      <c r="N84" s="29"/>
-      <c r="O84" s="29"/>
-      <c r="P84" s="27"/>
-      <c r="Q84" s="29"/>
-      <c r="R84" s="29"/>
-      <c r="S84" s="29"/>
+      <c r="H84" s="20"/>
+      <c r="I84" s="20"/>
+      <c r="J84" s="20"/>
+      <c r="K84" s="20"/>
+      <c r="L84" s="20"/>
+      <c r="M84" s="20"/>
+      <c r="N84" s="20"/>
+      <c r="O84" s="20"/>
+      <c r="P84" s="18"/>
+      <c r="Q84" s="20"/>
+      <c r="R84" s="20"/>
+      <c r="S84" s="20"/>
     </row>
     <row r="85" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G85" s="28">
+      <c r="G85" s="19">
         <v>45979</v>
       </c>
-      <c r="H85" s="29"/>
-      <c r="I85" s="29"/>
-      <c r="J85" s="29"/>
-      <c r="K85" s="29"/>
-      <c r="L85" s="29"/>
-      <c r="M85" s="29"/>
-      <c r="N85" s="29"/>
-      <c r="O85" s="29"/>
-      <c r="P85" s="27"/>
-      <c r="Q85" s="29"/>
-      <c r="R85" s="29"/>
-      <c r="S85" s="29"/>
+      <c r="H85" s="20"/>
+      <c r="I85" s="20"/>
+      <c r="J85" s="20"/>
+      <c r="K85" s="20"/>
+      <c r="L85" s="20"/>
+      <c r="M85" s="20"/>
+      <c r="N85" s="20"/>
+      <c r="O85" s="20"/>
+      <c r="P85" s="18"/>
+      <c r="Q85" s="20"/>
+      <c r="R85" s="20"/>
+      <c r="S85" s="20"/>
     </row>
     <row r="86" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G86" s="28">
+      <c r="G86" s="19">
         <v>45980</v>
       </c>
-      <c r="H86" s="29"/>
-      <c r="I86" s="29"/>
-      <c r="J86" s="29"/>
-      <c r="K86" s="29"/>
-      <c r="L86" s="29"/>
-      <c r="M86" s="29"/>
-      <c r="N86" s="29"/>
-      <c r="O86" s="29"/>
-      <c r="P86" s="27"/>
-      <c r="Q86" s="29"/>
-      <c r="R86" s="29"/>
-      <c r="S86" s="29"/>
+      <c r="H86" s="20"/>
+      <c r="I86" s="20"/>
+      <c r="J86" s="20"/>
+      <c r="K86" s="20"/>
+      <c r="L86" s="20"/>
+      <c r="M86" s="20"/>
+      <c r="N86" s="20"/>
+      <c r="O86" s="20"/>
+      <c r="P86" s="18"/>
+      <c r="Q86" s="20"/>
+      <c r="R86" s="20"/>
+      <c r="S86" s="20"/>
     </row>
     <row r="87" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G87" s="28">
+      <c r="G87" s="19">
         <v>45981</v>
       </c>
-      <c r="H87" s="29"/>
-      <c r="I87" s="29"/>
-      <c r="J87" s="29"/>
-      <c r="K87" s="29"/>
-      <c r="L87" s="29"/>
-      <c r="M87" s="29"/>
-      <c r="N87" s="29"/>
-      <c r="O87" s="29"/>
-      <c r="P87" s="27"/>
-      <c r="Q87" s="29"/>
-      <c r="R87" s="29"/>
-      <c r="S87" s="29"/>
+      <c r="H87" s="20"/>
+      <c r="I87" s="20"/>
+      <c r="J87" s="20"/>
+      <c r="K87" s="20"/>
+      <c r="L87" s="20"/>
+      <c r="M87" s="20"/>
+      <c r="N87" s="20"/>
+      <c r="O87" s="20"/>
+      <c r="P87" s="18"/>
+      <c r="Q87" s="20"/>
+      <c r="R87" s="20"/>
+      <c r="S87" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>